<commit_message>
Abrir Excel desde macOs en IberiaPay
</commit_message>
<xml_diff>
--- a/ErroresPruebas.xlsx
+++ b/ErroresPruebas.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="307">
   <si>
     <t>FECHA ERROR</t>
   </si>
@@ -533,6 +533,492 @@
   </si>
   <si>
     <t>GW-1595507573361-V4EHv</t>
+  </si>
+  <si>
+    <t>25/07/2020 01:14:17 +02</t>
+  </si>
+  <si>
+    <t>GW-1595632396026-V3amu</t>
+  </si>
+  <si>
+    <t>TIME-OUT</t>
+  </si>
+  <si>
+    <t>Tipo de Pago = CASH
+exception: {
+     stackTrace: com.ib.captwo.ndc.dist.coreservice.exceptions.NDCRepositoryException: java.net.SocketTimeoutException: SocketTimeoutException invoking http://ibissrva.corp.iberia.es/sse-orm/rs/v2/issue: Read timed out
+     errorCode: NDC_DIST_9009
+     errorDescription: 
+}</t>
+  </si>
+  <si>
+    <t>25/07/2020 02:56:14 +02</t>
+  </si>
+  <si>
+    <t>GW-1595638514079-JpZQi</t>
+  </si>
+  <si>
+    <t>25/07/2020 06:33:17 +02</t>
+  </si>
+  <si>
+    <t>GW-1595651536515-fSAKP</t>
+  </si>
+  <si>
+    <t>25/07/2020 08:29:18 +02</t>
+  </si>
+  <si>
+    <t>GW-1595658558295-L6LCz</t>
+  </si>
+  <si>
+    <t>NDC_DIST_2161</t>
+  </si>
+  <si>
+    <t>Payer's complete name should have a maximum length of 50 characters</t>
+  </si>
+  <si>
+    <t>25/07/2020 08:34:52 +02</t>
+  </si>
+  <si>
+    <t>GW-1595658831708-67fAj</t>
+  </si>
+  <si>
+    <t>25/07/2020 09:54:37 +02</t>
+  </si>
+  <si>
+    <t>GW-1595663612171-zNowM</t>
+  </si>
+  <si>
+    <t>25/07/2020 10:07:41 +02</t>
+  </si>
+  <si>
+    <t>GW-1595664400636-pvmUs</t>
+  </si>
+  <si>
+    <t>25/07/2020 10:09:07 +02</t>
+  </si>
+  <si>
+    <t>GW-1595664487225-ZvuuK</t>
+  </si>
+  <si>
+    <t>25/07/2020 10:47:43 +02</t>
+  </si>
+  <si>
+    <t>GW-1595666802883-3PinX</t>
+  </si>
+  <si>
+    <t>25/07/2020 11:28:34 +02</t>
+  </si>
+  <si>
+    <t>GW-1595669253887-cY0k7</t>
+  </si>
+  <si>
+    <t>25/07/2020 11:51:58 +02</t>
+  </si>
+  <si>
+    <t>GW-1595670657475-wgMa2</t>
+  </si>
+  <si>
+    <t>25/07/2020 12:10:00 +02</t>
+  </si>
+  <si>
+    <t>GW-1595671739777-vR6zz</t>
+  </si>
+  <si>
+    <t>25/07/2020 12:20:22 +02</t>
+  </si>
+  <si>
+    <t>GW-1595672361873-FzosA</t>
+  </si>
+  <si>
+    <t>25/07/2020 12:47:52 +02</t>
+  </si>
+  <si>
+    <t>GW-1595674011536-dipQq</t>
+  </si>
+  <si>
+    <t>25/07/2020 12:48:56 +02</t>
+  </si>
+  <si>
+    <t>GW-1595674076309-rSewJ</t>
+  </si>
+  <si>
+    <t>25/07/2020 13:12:26 +02</t>
+  </si>
+  <si>
+    <t>GW-1595675485412-bmxlu</t>
+  </si>
+  <si>
+    <t>25/07/2020 14:07:12 +02</t>
+  </si>
+  <si>
+    <t>GW-1595678772435-36bQ3</t>
+  </si>
+  <si>
+    <t>25/07/2020 14:21:26 +02</t>
+  </si>
+  <si>
+    <t>GW-1595679626005-tUOB6</t>
+  </si>
+  <si>
+    <t>25/07/2020 14:25:40 +02</t>
+  </si>
+  <si>
+    <t>GW-1595679879687-GQnPM</t>
+  </si>
+  <si>
+    <t>25/07/2020 15:09:19 +02</t>
+  </si>
+  <si>
+    <t>GW-1595682498603-mPW9f</t>
+  </si>
+  <si>
+    <t>25/07/2020 15:26:10 +02</t>
+  </si>
+  <si>
+    <t>GW-1595683509472-GtkIj</t>
+  </si>
+  <si>
+    <t>25/07/2020 15:48:57 +02</t>
+  </si>
+  <si>
+    <t>GW-1595684876991-ZK25E</t>
+  </si>
+  <si>
+    <t>25/07/2020 17:02:49 +02</t>
+  </si>
+  <si>
+    <t>GW-1595689305261-mzfzJ</t>
+  </si>
+  <si>
+    <t>25/07/2020 17:29:13 +02</t>
+  </si>
+  <si>
+    <t>GW-1595690892911-6jhjd</t>
+  </si>
+  <si>
+    <t>25/07/2020 17:40:48 +02</t>
+  </si>
+  <si>
+    <t>GW-1595691588134-XE8Gh</t>
+  </si>
+  <si>
+    <t>25/07/2020 18:29:12 +02</t>
+  </si>
+  <si>
+    <t>GW-1595694492351-dWs8y</t>
+  </si>
+  <si>
+    <t>25/07/2020 19:35:32 +02</t>
+  </si>
+  <si>
+    <t>GW-1595698472126-1ozR4</t>
+  </si>
+  <si>
+    <t>25/07/2020 19:50:20 +02</t>
+  </si>
+  <si>
+    <t>GW-1595699359786-fEflf</t>
+  </si>
+  <si>
+    <t>25/07/2020 20:03:18 +02</t>
+  </si>
+  <si>
+    <t>GW-1595700138243-gOeZ0</t>
+  </si>
+  <si>
+    <t>25/07/2020 20:53:14 +02</t>
+  </si>
+  <si>
+    <t>GW-1595703132785-QXoQU</t>
+  </si>
+  <si>
+    <t>25/07/2020 22:21:28 +02</t>
+  </si>
+  <si>
+    <t>GW-1595708428212-3LPGT</t>
+  </si>
+  <si>
+    <t>25/07/2020 22:46:01 +02</t>
+  </si>
+  <si>
+    <t>GW-1595709901028-Hq3v4</t>
+  </si>
+  <si>
+    <t>25/07/2020 23:41:54 +02</t>
+  </si>
+  <si>
+    <t>GW-1595713254060-jIxEO</t>
+  </si>
+  <si>
+    <t>25/07/2020 02:37:07 +02</t>
+  </si>
+  <si>
+    <t>GW-1595637363239-Xir2Z</t>
+  </si>
+  <si>
+    <t>Tipo de Pago = CREDIT_CARD
+PNR = JVS78  | FRAUDE: 100 - ACCEPT  | TRANSACCION: 00000000238759  | PAGO: PAID (OK - Completion without incidents.)</t>
+  </si>
+  <si>
+    <t>25/07/2020 04:45:03 +02</t>
+  </si>
+  <si>
+    <t>GW-1595645039423-mMc7a</t>
+  </si>
+  <si>
+    <t>Tipo de Pago = CREDIT_CARD
+PNR = JVSN0  | FRAUDE: 100 - ACCEPT  | TRANSACCION: 00000000238811  | PAGO: PAID (OK - Completion without incidents.)</t>
+  </si>
+  <si>
+    <t>25/07/2020 09:22:02 +02</t>
+  </si>
+  <si>
+    <t>GW-1595661712287-IYRCe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si è verificato un errore di pagamento durante la prenotazione.
+</t>
+  </si>
+  <si>
+    <t>JVTNH | (WCS - CircuitBreaker) PAC_UTILS_E0006 - CONTENTS_ERROR</t>
+  </si>
+  <si>
+    <t>25/07/2020 09:26:36 +02</t>
+  </si>
+  <si>
+    <t>GW-1595661934876-iUfPu</t>
+  </si>
+  <si>
+    <t>25/07/2020 09:51:57 +02</t>
+  </si>
+  <si>
+    <t>GW-1595663506115-qtgrh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ocorreu um erro com o pagamento no momento da reserva.
+</t>
+  </si>
+  <si>
+    <t>JVTXK | (WCS - CircuitBreaker) PAC_UTILS_E0006 - CONTENTS_ERROR</t>
+  </si>
+  <si>
+    <t>25/07/2020 11:54:37 +02</t>
+  </si>
+  <si>
+    <t>GW-1595670810159-Q32VN</t>
+  </si>
+  <si>
+    <t>25/07/2020 12:57:33 +02</t>
+  </si>
+  <si>
+    <t>GW-1595674587202-RcQCD</t>
+  </si>
+  <si>
+    <t>25/07/2020 13:18:14 +02</t>
+  </si>
+  <si>
+    <t>GW-1595675894241-evlTH</t>
+  </si>
+  <si>
+    <t>421 - NOT AVAILABLE AND WAITLIST IS CLOSED'
+FlightPrice/OfferPrice ejecutado aprox. : 25/07/2020 13:18:11 +02
+Slice 1:
+F1: IB768820200727 LCY-IBZ &gt; BA - British Airways &amp; Clase K (3 asientos libres)</t>
+  </si>
+  <si>
+    <t>25/07/2020 13:44:16 +02</t>
+  </si>
+  <si>
+    <t>GW-1595677395539-mvI8o</t>
+  </si>
+  <si>
+    <t>25/07/2020 14:12:50 +02</t>
+  </si>
+  <si>
+    <t>GW-1595679106789-jh8dk</t>
+  </si>
+  <si>
+    <t>25/07/2020 14:35:00 +02</t>
+  </si>
+  <si>
+    <t>GW-1595680438482-7Fu4g</t>
+  </si>
+  <si>
+    <t>25/07/2020 15:59:58 +02</t>
+  </si>
+  <si>
+    <t>GW-1595685535266-dPS8P</t>
+  </si>
+  <si>
+    <t>25/07/2020 17:11:56 +02</t>
+  </si>
+  <si>
+    <t>GW-1595689854416-cgMrf</t>
+  </si>
+  <si>
+    <t>25/07/2020 17:25:02 +02</t>
+  </si>
+  <si>
+    <t>GW-1595690634440-tbMyh</t>
+  </si>
+  <si>
+    <t>Tipo de Pago = CREDIT_CARD
+PNR = MW99G  | FRAUDE: 100 - ACCEPT  | TRANSACCION: 00000000239852  | PAGO: PAID (OK - Completion without incidents.)</t>
+  </si>
+  <si>
+    <t>25/07/2020 19:25:11 +02</t>
+  </si>
+  <si>
+    <t>GW-1595697840109-2MG7S</t>
+  </si>
+  <si>
+    <t>25/07/2020 20:47:02 +02</t>
+  </si>
+  <si>
+    <t>GW-1595702760973-egQJm</t>
+  </si>
+  <si>
+    <t>Tipo de Pago = CREDIT_CARD
+PNR = HY05L  | FRAUDE: 480 - REVIEW  | TRANSACCION: 00000000240307  | PAGO: PAID (OK - Completion without incidents.)</t>
+  </si>
+  <si>
+    <t>25/07/2020 20:55:05 +02</t>
+  </si>
+  <si>
+    <t>GW-1595703243780-1xCSa</t>
+  </si>
+  <si>
+    <t>Tipo de Pago = CREDIT_CARD
+PNR = HY08K  | FRAUDE: 480 - REVIEW  | TRANSACCION: 00000000240328  | PAGO: PAID (OK - Completion without incidents.)</t>
+  </si>
+  <si>
+    <t>25/07/2020 20:57:43 +02</t>
+  </si>
+  <si>
+    <t>GW-1595703399844-XG4P9</t>
+  </si>
+  <si>
+    <t>25/07/2020 21:04:47 +02</t>
+  </si>
+  <si>
+    <t>GW-1595703824593-N9WAM</t>
+  </si>
+  <si>
+    <t>25/07/2020 21:28:35 +02</t>
+  </si>
+  <si>
+    <t>GW-1595705253946-mz5Ah</t>
+  </si>
+  <si>
+    <t>Tipo de Pago = CREDIT_CARD
+PNR = HY0PS  | FRAUDE: 100 - ACCEPT  | TRANSACCION: 00000000240403  | PAGO: PAID (OK - Completion without incidents.)</t>
+  </si>
+  <si>
+    <t>25/07/2020 23:26:45 +02</t>
+  </si>
+  <si>
+    <t>GW-1595712405596-ltU0o</t>
+  </si>
+  <si>
+    <t>421 - NOT AVAILABLE AND WAITLIST IS CLOSED'
+FlightPrice/OfferPrice ejecutado aprox. : 25/07/2020 23:26:44 +02
+Slice 1:
+F1: IB268220201024 PTP-ORY &gt; o0 - LEVEL operado por Openskies &amp; Clase Q (9 asientos libres)
+Slice 2:
+F1: IB268120201029 ORY-PTP &gt; o0 - LEVEL operado por Openskies &amp; Clase A (9 asientos libres)</t>
+  </si>
+  <si>
+    <t>25/07/2020 23:30:36 +02</t>
+  </si>
+  <si>
+    <t>GW-1595712636417-4of1d</t>
+  </si>
+  <si>
+    <t>421 - NOT AVAILABLE AND WAITLIST IS CLOSED'
+FlightPrice/OfferPrice ejecutado aprox. : 25/07/2020 23:30:34 +02
+Slice 1:
+F1: IB268220201024 PTP-ORY &gt; o0 - LEVEL operado por Openskies &amp; Clase Q (9 asientos libres)
+Slice 2:
+F1: IB268120201029 ORY-PTP &gt; o0 - LEVEL operado por Openskies &amp; Clase A (9 asientos libres)</t>
+  </si>
+  <si>
+    <t>27/07/2020 02:45:33 +02</t>
+  </si>
+  <si>
+    <t>GW-1595810727177-EnHbt</t>
+  </si>
+  <si>
+    <t>ASS_FASS_409</t>
+  </si>
+  <si>
+    <t>Ancillaries sell failure.</t>
+  </si>
+  <si>
+    <t>27/07/2020 04:28:28 +02</t>
+  </si>
+  <si>
+    <t>GW-1595816847408-N9XWD</t>
+  </si>
+  <si>
+    <t>27/07/2020 06:31:32 +02</t>
+  </si>
+  <si>
+    <t>GW-1595824231323-43fOn</t>
+  </si>
+  <si>
+    <t>Tipo de Pago = CREDIT_CARD
+PNR = LPJP8  | FRAUDE: 100 - ACCEPT  | TRANSACCION: 00000000242954  | PAGO: PAID (OK - Completion without incidents.)</t>
+  </si>
+  <si>
+    <t>27/07/2020 08:59:12 +02</t>
+  </si>
+  <si>
+    <t>GW-1595833091506-PRPBi</t>
+  </si>
+  <si>
+    <t>Tipo de Pago = CREDIT_CARD
+PNR = LPKHH  | FRAUDE: 100 - ACCEPT  | TRANSACCION: 00000000243025  | PAGO: PAID (OK - Completion without incidents.)</t>
+  </si>
+  <si>
+    <t>27/07/2020 09:56:57 +02</t>
+  </si>
+  <si>
+    <t>GW-1595836550115-KWzG5</t>
+  </si>
+  <si>
+    <t>Tipo de Pago = CREDIT_CARD
+PNR = LPLDS  | FRAUDE: 100 - ACCEPT  | TRANSACCION: 00000000243105  | PAGO: PAID (OK - Completion without incidents.)</t>
+  </si>
+  <si>
+    <t>27/07/2020 09:59:10 +02</t>
+  </si>
+  <si>
+    <t>GW-1595836745656-8qoeU</t>
+  </si>
+  <si>
+    <t>LPLG3 | (WCS - CircuitBreaker) PAC_UTILS_E0006 - CONTENTS_ERROR</t>
+  </si>
+  <si>
+    <t>27/07/2020 10:15:44 +02</t>
+  </si>
+  <si>
+    <t>GW-1595837683904-0P7F2</t>
+  </si>
+  <si>
+    <t>Tipo de Pago = CREDIT_CARD
+PNR = LPLSM  | FRAUDE: 480 - REVIEW  | TRANSACCION: 00000000243157  | PAGO: PAID (OK - Completion without incidents.)</t>
+  </si>
+  <si>
+    <t>27/07/2020 10:16:21 +02</t>
+  </si>
+  <si>
+    <t>GW-1595837718844-GDETV</t>
+  </si>
+  <si>
+    <t>27/07/2020 11:48:39 +02</t>
+  </si>
+  <si>
+    <t>GW-1595843255619-2bDoK</t>
   </si>
 </sst>
 </file>
@@ -595,7 +1081,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -984,6 +1470,30 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true" vertical="center"/>
@@ -1983,7 +2493,7 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -2113,6 +2623,765 @@
       </c>
       <c r="G6" s="130" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="137" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="137" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="137" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F8" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G8" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="137" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9" s="137" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F9" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G9" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="137" t="s">
+        <v>161</v>
+      </c>
+      <c r="B10" s="137" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="E10" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F10" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G10" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="137" t="s">
+        <v>163</v>
+      </c>
+      <c r="B11" s="137" t="s">
+        <v>164</v>
+      </c>
+      <c r="C11" s="137" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="137" t="s">
+        <v>166</v>
+      </c>
+      <c r="E11" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F11" s="137" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="137" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="137" t="s">
+        <v>167</v>
+      </c>
+      <c r="B12" s="137" t="s">
+        <v>168</v>
+      </c>
+      <c r="C12" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F12" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G12" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="137" t="s">
+        <v>169</v>
+      </c>
+      <c r="B13" s="137" t="s">
+        <v>170</v>
+      </c>
+      <c r="C13" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" s="137" t="s">
+        <v>120</v>
+      </c>
+      <c r="E13" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F13" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G13" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="137" t="s">
+        <v>171</v>
+      </c>
+      <c r="B14" s="137" t="s">
+        <v>172</v>
+      </c>
+      <c r="C14" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="E14" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F14" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G14" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="137" t="s">
+        <v>173</v>
+      </c>
+      <c r="B15" s="137" t="s">
+        <v>174</v>
+      </c>
+      <c r="C15" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" s="137" t="s">
+        <v>120</v>
+      </c>
+      <c r="E15" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F15" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G15" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="137" t="s">
+        <v>175</v>
+      </c>
+      <c r="B16" s="137" t="s">
+        <v>176</v>
+      </c>
+      <c r="C16" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F16" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G16" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="137" t="s">
+        <v>177</v>
+      </c>
+      <c r="B17" s="137" t="s">
+        <v>178</v>
+      </c>
+      <c r="C17" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="137" t="s">
+        <v>120</v>
+      </c>
+      <c r="E17" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F17" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G17" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="137" t="s">
+        <v>179</v>
+      </c>
+      <c r="B18" s="137" t="s">
+        <v>180</v>
+      </c>
+      <c r="C18" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="E18" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F18" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G18" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="137" t="s">
+        <v>181</v>
+      </c>
+      <c r="B19" s="137" t="s">
+        <v>182</v>
+      </c>
+      <c r="C19" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="E19" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F19" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G19" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="137" t="s">
+        <v>183</v>
+      </c>
+      <c r="B20" s="137" t="s">
+        <v>184</v>
+      </c>
+      <c r="C20" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="E20" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F20" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G20" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="137" t="s">
+        <v>185</v>
+      </c>
+      <c r="B21" s="137" t="s">
+        <v>186</v>
+      </c>
+      <c r="C21" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D21" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F21" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G21" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="137" t="s">
+        <v>187</v>
+      </c>
+      <c r="B22" s="137" t="s">
+        <v>188</v>
+      </c>
+      <c r="C22" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="E22" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F22" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G22" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="137" t="s">
+        <v>189</v>
+      </c>
+      <c r="B23" s="137" t="s">
+        <v>190</v>
+      </c>
+      <c r="C23" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="137" t="s">
+        <v>120</v>
+      </c>
+      <c r="E23" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F23" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G23" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="137" t="s">
+        <v>191</v>
+      </c>
+      <c r="B24" s="137" t="s">
+        <v>192</v>
+      </c>
+      <c r="C24" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="E24" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F24" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G24" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="137" t="s">
+        <v>193</v>
+      </c>
+      <c r="B25" s="137" t="s">
+        <v>194</v>
+      </c>
+      <c r="C25" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="E25" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F25" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G25" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="137" t="s">
+        <v>195</v>
+      </c>
+      <c r="B26" s="137" t="s">
+        <v>196</v>
+      </c>
+      <c r="C26" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F26" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G26" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="137" t="s">
+        <v>197</v>
+      </c>
+      <c r="B27" s="137" t="s">
+        <v>198</v>
+      </c>
+      <c r="C27" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="E27" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F27" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G27" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="137" t="s">
+        <v>199</v>
+      </c>
+      <c r="B28" s="137" t="s">
+        <v>200</v>
+      </c>
+      <c r="C28" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F28" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G28" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="137" t="s">
+        <v>201</v>
+      </c>
+      <c r="B29" s="137" t="s">
+        <v>202</v>
+      </c>
+      <c r="C29" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="E29" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F29" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G29" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="137" t="s">
+        <v>203</v>
+      </c>
+      <c r="B30" s="137" t="s">
+        <v>204</v>
+      </c>
+      <c r="C30" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" s="137" t="s">
+        <v>120</v>
+      </c>
+      <c r="E30" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F30" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G30" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="137" t="s">
+        <v>205</v>
+      </c>
+      <c r="B31" s="137" t="s">
+        <v>206</v>
+      </c>
+      <c r="C31" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" s="137" t="s">
+        <v>120</v>
+      </c>
+      <c r="E31" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F31" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G31" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="137" t="s">
+        <v>207</v>
+      </c>
+      <c r="B32" s="137" t="s">
+        <v>208</v>
+      </c>
+      <c r="C32" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="E32" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F32" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G32" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="137" t="s">
+        <v>209</v>
+      </c>
+      <c r="B33" s="137" t="s">
+        <v>210</v>
+      </c>
+      <c r="C33" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="E33" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F33" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G33" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="137" t="s">
+        <v>211</v>
+      </c>
+      <c r="B34" s="137" t="s">
+        <v>212</v>
+      </c>
+      <c r="C34" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="E34" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F34" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G34" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="137" t="s">
+        <v>213</v>
+      </c>
+      <c r="B35" s="137" t="s">
+        <v>214</v>
+      </c>
+      <c r="C35" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="E35" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F35" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G35" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="137" t="s">
+        <v>215</v>
+      </c>
+      <c r="B36" s="137" t="s">
+        <v>216</v>
+      </c>
+      <c r="C36" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="E36" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F36" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G36" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="137" t="s">
+        <v>217</v>
+      </c>
+      <c r="B37" s="137" t="s">
+        <v>218</v>
+      </c>
+      <c r="C37" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37" s="137" t="s">
+        <v>120</v>
+      </c>
+      <c r="E37" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F37" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G37" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="137" t="s">
+        <v>219</v>
+      </c>
+      <c r="B38" s="137" t="s">
+        <v>220</v>
+      </c>
+      <c r="C38" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="137" t="s">
+        <v>120</v>
+      </c>
+      <c r="E38" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F38" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G38" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="137" t="s">
+        <v>221</v>
+      </c>
+      <c r="B39" s="137" t="s">
+        <v>222</v>
+      </c>
+      <c r="C39" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D39" s="137" t="s">
+        <v>120</v>
+      </c>
+      <c r="E39" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F39" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G39" s="137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="137" t="s">
+        <v>223</v>
+      </c>
+      <c r="B40" s="137" t="s">
+        <v>224</v>
+      </c>
+      <c r="C40" s="137" t="s">
+        <v>112</v>
+      </c>
+      <c r="D40" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="E40" s="138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F40" s="137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G40" s="137" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2936,7 +4205,7 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -3638,6 +4907,903 @@
         <v>21</v>
       </c>
       <c r="G31" s="135" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="139" t="s">
+        <v>225</v>
+      </c>
+      <c r="B33" s="139" t="s">
+        <v>226</v>
+      </c>
+      <c r="C33" s="139" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" s="139" t="s">
+        <v>113</v>
+      </c>
+      <c r="E33" s="140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F33" s="139" t="s">
+        <v>21</v>
+      </c>
+      <c r="G33" s="139" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="139" t="s">
+        <v>228</v>
+      </c>
+      <c r="B34" s="139" t="s">
+        <v>229</v>
+      </c>
+      <c r="C34" s="139" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" s="139" t="s">
+        <v>113</v>
+      </c>
+      <c r="E34" s="140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F34" s="139" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" s="139" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="139" t="s">
+        <v>231</v>
+      </c>
+      <c r="B35" s="139" t="s">
+        <v>232</v>
+      </c>
+      <c r="C35" s="139" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="139" t="s">
+        <v>233</v>
+      </c>
+      <c r="E35" s="140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F35" s="139" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35" s="139" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="139" t="s">
+        <v>235</v>
+      </c>
+      <c r="B36" s="139" t="s">
+        <v>236</v>
+      </c>
+      <c r="C36" s="139" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" s="139" t="s">
+        <v>113</v>
+      </c>
+      <c r="E36" s="140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F36" s="139" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" s="139" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="139" t="s">
+        <v>237</v>
+      </c>
+      <c r="B37" s="139" t="s">
+        <v>238</v>
+      </c>
+      <c r="C37" s="139" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="139" t="s">
+        <v>239</v>
+      </c>
+      <c r="E37" s="140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F37" s="139" t="s">
+        <v>24</v>
+      </c>
+      <c r="G37" s="139" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="139" t="s">
+        <v>241</v>
+      </c>
+      <c r="B38" s="139" t="s">
+        <v>242</v>
+      </c>
+      <c r="C38" s="139" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="139" t="s">
+        <v>120</v>
+      </c>
+      <c r="E38" s="140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F38" s="139" t="s">
+        <v>21</v>
+      </c>
+      <c r="G38" s="139" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="139" t="s">
+        <v>243</v>
+      </c>
+      <c r="B39" s="139" t="s">
+        <v>244</v>
+      </c>
+      <c r="C39" s="139" t="s">
+        <v>112</v>
+      </c>
+      <c r="D39" s="139" t="s">
+        <v>120</v>
+      </c>
+      <c r="E39" s="140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F39" s="139" t="s">
+        <v>21</v>
+      </c>
+      <c r="G39" s="139" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="139" t="s">
+        <v>245</v>
+      </c>
+      <c r="B40" s="139" t="s">
+        <v>246</v>
+      </c>
+      <c r="C40" s="139" t="s">
+        <v>128</v>
+      </c>
+      <c r="D40" s="139" t="s">
+        <v>129</v>
+      </c>
+      <c r="E40" s="140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F40" s="139" t="s">
+        <v>21</v>
+      </c>
+      <c r="G40" s="139" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="139" t="s">
+        <v>248</v>
+      </c>
+      <c r="B41" s="139" t="s">
+        <v>249</v>
+      </c>
+      <c r="C41" s="139" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" s="139" t="s">
+        <v>120</v>
+      </c>
+      <c r="E41" s="140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F41" s="139" t="s">
+        <v>21</v>
+      </c>
+      <c r="G41" s="139" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="139" t="s">
+        <v>250</v>
+      </c>
+      <c r="B42" s="139" t="s">
+        <v>251</v>
+      </c>
+      <c r="C42" s="139" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42" s="139" t="s">
+        <v>113</v>
+      </c>
+      <c r="E42" s="140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F42" s="139" t="s">
+        <v>21</v>
+      </c>
+      <c r="G42" s="139" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="139" t="s">
+        <v>252</v>
+      </c>
+      <c r="B43" s="139" t="s">
+        <v>253</v>
+      </c>
+      <c r="C43" s="139" t="s">
+        <v>112</v>
+      </c>
+      <c r="D43" s="139" t="s">
+        <v>120</v>
+      </c>
+      <c r="E43" s="140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F43" s="139" t="s">
+        <v>21</v>
+      </c>
+      <c r="G43" s="139" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="139" t="s">
+        <v>254</v>
+      </c>
+      <c r="B44" s="139" t="s">
+        <v>255</v>
+      </c>
+      <c r="C44" s="139" t="s">
+        <v>112</v>
+      </c>
+      <c r="D44" s="139" t="s">
+        <v>113</v>
+      </c>
+      <c r="E44" s="140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F44" s="139" t="s">
+        <v>21</v>
+      </c>
+      <c r="G44" s="139" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="139" t="s">
+        <v>256</v>
+      </c>
+      <c r="B45" s="139" t="s">
+        <v>257</v>
+      </c>
+      <c r="C45" s="139" t="s">
+        <v>112</v>
+      </c>
+      <c r="D45" s="139" t="s">
+        <v>120</v>
+      </c>
+      <c r="E45" s="140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F45" s="139" t="s">
+        <v>21</v>
+      </c>
+      <c r="G45" s="139" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="139" t="s">
+        <v>258</v>
+      </c>
+      <c r="B46" s="139" t="s">
+        <v>259</v>
+      </c>
+      <c r="C46" s="139" t="s">
+        <v>112</v>
+      </c>
+      <c r="D46" s="139" t="s">
+        <v>113</v>
+      </c>
+      <c r="E46" s="140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F46" s="139" t="s">
+        <v>21</v>
+      </c>
+      <c r="G46" s="139" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="139" t="s">
+        <v>261</v>
+      </c>
+      <c r="B47" s="139" t="s">
+        <v>262</v>
+      </c>
+      <c r="C47" s="139" t="s">
+        <v>112</v>
+      </c>
+      <c r="D47" s="139" t="s">
+        <v>120</v>
+      </c>
+      <c r="E47" s="140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F47" s="139" t="s">
+        <v>21</v>
+      </c>
+      <c r="G47" s="139" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="139" t="s">
+        <v>263</v>
+      </c>
+      <c r="B48" s="139" t="s">
+        <v>264</v>
+      </c>
+      <c r="C48" s="139" t="s">
+        <v>112</v>
+      </c>
+      <c r="D48" s="139" t="s">
+        <v>113</v>
+      </c>
+      <c r="E48" s="140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F48" s="139" t="s">
+        <v>21</v>
+      </c>
+      <c r="G48" s="139" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="139" t="s">
+        <v>266</v>
+      </c>
+      <c r="B49" s="139" t="s">
+        <v>267</v>
+      </c>
+      <c r="C49" s="139" t="s">
+        <v>112</v>
+      </c>
+      <c r="D49" s="139" t="s">
+        <v>113</v>
+      </c>
+      <c r="E49" s="140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F49" s="139" t="s">
+        <v>21</v>
+      </c>
+      <c r="G49" s="139" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="139" t="s">
+        <v>269</v>
+      </c>
+      <c r="B50" s="139" t="s">
+        <v>270</v>
+      </c>
+      <c r="C50" s="139" t="s">
+        <v>112</v>
+      </c>
+      <c r="D50" s="139" t="s">
+        <v>120</v>
+      </c>
+      <c r="E50" s="140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F50" s="139" t="s">
+        <v>21</v>
+      </c>
+      <c r="G50" s="139" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="139" t="s">
+        <v>271</v>
+      </c>
+      <c r="B51" s="139" t="s">
+        <v>272</v>
+      </c>
+      <c r="C51" s="139" t="s">
+        <v>112</v>
+      </c>
+      <c r="D51" s="139" t="s">
+        <v>120</v>
+      </c>
+      <c r="E51" s="140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F51" s="139" t="s">
+        <v>21</v>
+      </c>
+      <c r="G51" s="139" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="139" t="s">
+        <v>273</v>
+      </c>
+      <c r="B52" s="139" t="s">
+        <v>274</v>
+      </c>
+      <c r="C52" s="139" t="s">
+        <v>112</v>
+      </c>
+      <c r="D52" s="139" t="s">
+        <v>113</v>
+      </c>
+      <c r="E52" s="140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F52" s="139" t="s">
+        <v>21</v>
+      </c>
+      <c r="G52" s="139" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="139" t="s">
+        <v>276</v>
+      </c>
+      <c r="B53" s="139" t="s">
+        <v>277</v>
+      </c>
+      <c r="C53" s="139" t="s">
+        <v>128</v>
+      </c>
+      <c r="D53" s="139" t="s">
+        <v>129</v>
+      </c>
+      <c r="E53" s="140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F53" s="139" t="s">
+        <v>21</v>
+      </c>
+      <c r="G53" s="139" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="139" t="s">
+        <v>279</v>
+      </c>
+      <c r="B54" s="139" t="s">
+        <v>280</v>
+      </c>
+      <c r="C54" s="139" t="s">
+        <v>128</v>
+      </c>
+      <c r="D54" s="139" t="s">
+        <v>129</v>
+      </c>
+      <c r="E54" s="140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F54" s="139" t="s">
+        <v>21</v>
+      </c>
+      <c r="G54" s="139" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="141" t="s">
+        <v>282</v>
+      </c>
+      <c r="B56" s="141" t="s">
+        <v>283</v>
+      </c>
+      <c r="C56" s="141" t="s">
+        <v>284</v>
+      </c>
+      <c r="D56" s="141" t="s">
+        <v>285</v>
+      </c>
+      <c r="E56" s="142" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F56" s="141" t="s">
+        <v>21</v>
+      </c>
+      <c r="G56" s="141" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="141" t="s">
+        <v>286</v>
+      </c>
+      <c r="B57" s="141" t="s">
+        <v>287</v>
+      </c>
+      <c r="C57" s="141" t="s">
+        <v>112</v>
+      </c>
+      <c r="D57" s="141" t="s">
+        <v>120</v>
+      </c>
+      <c r="E57" s="142" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F57" s="141" t="s">
+        <v>21</v>
+      </c>
+      <c r="G57" s="141" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="141" t="s">
+        <v>288</v>
+      </c>
+      <c r="B58" s="141" t="s">
+        <v>289</v>
+      </c>
+      <c r="C58" s="141" t="s">
+        <v>112</v>
+      </c>
+      <c r="D58" s="141" t="s">
+        <v>113</v>
+      </c>
+      <c r="E58" s="142" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F58" s="141" t="s">
+        <v>21</v>
+      </c>
+      <c r="G58" s="141" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="141" t="s">
+        <v>291</v>
+      </c>
+      <c r="B59" s="141" t="s">
+        <v>292</v>
+      </c>
+      <c r="C59" s="141" t="s">
+        <v>112</v>
+      </c>
+      <c r="D59" s="141" t="s">
+        <v>113</v>
+      </c>
+      <c r="E59" s="142" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F59" s="141" t="s">
+        <v>21</v>
+      </c>
+      <c r="G59" s="141" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="141" t="s">
+        <v>294</v>
+      </c>
+      <c r="B60" s="141" t="s">
+        <v>295</v>
+      </c>
+      <c r="C60" s="141" t="s">
+        <v>112</v>
+      </c>
+      <c r="D60" s="141" t="s">
+        <v>113</v>
+      </c>
+      <c r="E60" s="142" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F60" s="141" t="s">
+        <v>21</v>
+      </c>
+      <c r="G60" s="141" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="141" t="s">
+        <v>297</v>
+      </c>
+      <c r="B61" s="141" t="s">
+        <v>298</v>
+      </c>
+      <c r="C61" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="D61" s="141" t="s">
+        <v>239</v>
+      </c>
+      <c r="E61" s="142" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F61" s="141" t="s">
+        <v>24</v>
+      </c>
+      <c r="G61" s="141" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="141" t="s">
+        <v>300</v>
+      </c>
+      <c r="B62" s="141" t="s">
+        <v>301</v>
+      </c>
+      <c r="C62" s="141" t="s">
+        <v>112</v>
+      </c>
+      <c r="D62" s="141" t="s">
+        <v>113</v>
+      </c>
+      <c r="E62" s="142" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F62" s="141" t="s">
+        <v>21</v>
+      </c>
+      <c r="G62" s="141" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="141" t="s">
+        <v>303</v>
+      </c>
+      <c r="B63" s="141" t="s">
+        <v>304</v>
+      </c>
+      <c r="C63" s="141" t="s">
+        <v>112</v>
+      </c>
+      <c r="D63" s="141" t="s">
+        <v>120</v>
+      </c>
+      <c r="E63" s="142" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F63" s="141" t="s">
+        <v>21</v>
+      </c>
+      <c r="G63" s="141" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="143" t="s">
+        <v>282</v>
+      </c>
+      <c r="B65" s="143" t="s">
+        <v>283</v>
+      </c>
+      <c r="C65" s="143" t="s">
+        <v>284</v>
+      </c>
+      <c r="D65" s="143" t="s">
+        <v>285</v>
+      </c>
+      <c r="E65" s="144" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F65" s="143" t="s">
+        <v>21</v>
+      </c>
+      <c r="G65" s="143" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="143" t="s">
+        <v>286</v>
+      </c>
+      <c r="B66" s="143" t="s">
+        <v>287</v>
+      </c>
+      <c r="C66" s="143" t="s">
+        <v>112</v>
+      </c>
+      <c r="D66" s="143" t="s">
+        <v>120</v>
+      </c>
+      <c r="E66" s="144" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F66" s="143" t="s">
+        <v>21</v>
+      </c>
+      <c r="G66" s="143" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="143" t="s">
+        <v>288</v>
+      </c>
+      <c r="B67" s="143" t="s">
+        <v>289</v>
+      </c>
+      <c r="C67" s="143" t="s">
+        <v>112</v>
+      </c>
+      <c r="D67" s="143" t="s">
+        <v>113</v>
+      </c>
+      <c r="E67" s="144" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F67" s="143" t="s">
+        <v>21</v>
+      </c>
+      <c r="G67" s="143" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="143" t="s">
+        <v>291</v>
+      </c>
+      <c r="B68" s="143" t="s">
+        <v>292</v>
+      </c>
+      <c r="C68" s="143" t="s">
+        <v>112</v>
+      </c>
+      <c r="D68" s="143" t="s">
+        <v>113</v>
+      </c>
+      <c r="E68" s="144" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F68" s="143" t="s">
+        <v>21</v>
+      </c>
+      <c r="G68" s="143" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="143" t="s">
+        <v>294</v>
+      </c>
+      <c r="B69" s="143" t="s">
+        <v>295</v>
+      </c>
+      <c r="C69" s="143" t="s">
+        <v>112</v>
+      </c>
+      <c r="D69" s="143" t="s">
+        <v>113</v>
+      </c>
+      <c r="E69" s="144" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F69" s="143" t="s">
+        <v>21</v>
+      </c>
+      <c r="G69" s="143" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="143" t="s">
+        <v>297</v>
+      </c>
+      <c r="B70" s="143" t="s">
+        <v>298</v>
+      </c>
+      <c r="C70" s="143" t="s">
+        <v>23</v>
+      </c>
+      <c r="D70" s="143" t="s">
+        <v>239</v>
+      </c>
+      <c r="E70" s="144" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F70" s="143" t="s">
+        <v>24</v>
+      </c>
+      <c r="G70" s="143" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="143" t="s">
+        <v>300</v>
+      </c>
+      <c r="B71" s="143" t="s">
+        <v>301</v>
+      </c>
+      <c r="C71" s="143" t="s">
+        <v>112</v>
+      </c>
+      <c r="D71" s="143" t="s">
+        <v>113</v>
+      </c>
+      <c r="E71" s="144" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F71" s="143" t="s">
+        <v>21</v>
+      </c>
+      <c r="G71" s="143" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="143" t="s">
+        <v>303</v>
+      </c>
+      <c r="B72" s="143" t="s">
+        <v>304</v>
+      </c>
+      <c r="C72" s="143" t="s">
+        <v>112</v>
+      </c>
+      <c r="D72" s="143" t="s">
+        <v>120</v>
+      </c>
+      <c r="E72" s="144" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F72" s="143" t="s">
+        <v>21</v>
+      </c>
+      <c r="G72" s="143" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="143" t="s">
+        <v>305</v>
+      </c>
+      <c r="B73" s="143" t="s">
+        <v>306</v>
+      </c>
+      <c r="C73" s="143" t="s">
+        <v>112</v>
+      </c>
+      <c r="D73" s="143" t="s">
+        <v>113</v>
+      </c>
+      <c r="E73" s="144" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F73" s="143" t="s">
+        <v>21</v>
+      </c>
+      <c r="G73" s="143" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>